<commit_message>
fix: template guest book
</commit_message>
<xml_diff>
--- a/src/assets/excel/buku_tamu.xlsx
+++ b/src/assets/excel/buku_tamu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rendi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A062081D-D1E6-480D-A94F-1340F07E1632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE5FD15-B59D-445E-BC65-9DB479219609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E286C7BD-9FE2-4A9A-849D-A4A6F0B60E12}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>no</t>
   </si>
@@ -80,6 +80,18 @@
   </si>
   <si>
     <t>keluarga</t>
+  </si>
+  <si>
+    <t>sesi</t>
+  </si>
+  <si>
+    <t>Irham</t>
+  </si>
+  <si>
+    <t>Bogor</t>
+  </si>
+  <si>
+    <t>082111002299</t>
   </si>
 </sst>
 </file>
@@ -432,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB30828-C56D-4BC0-A419-42043EF5049B}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +459,7 @@
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,8 +475,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -480,8 +495,11 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -497,8 +515,11 @@
       <c r="E3" t="s">
         <v>12</v>
       </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -513,6 +534,29 @@
       </c>
       <c r="E4" t="s">
         <v>15</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>